<commit_message>
adjusted personnel sheet to fix EML validation errors
</commit_message>
<xml_diff>
--- a/nes-lter-events-transect-info.xlsx
+++ b/nes-lter-events-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-events-transect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfutrelle\Documents\GitHub\nes-lter-events-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96C0C85-6E99-4C1A-8522-61138C88CE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF45EB3-1837-42F1-9A37-FAD4AB724896}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29115" yWindow="1035" windowWidth="25095" windowHeight="18765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29118" yWindow="1038" windowWidth="25098" windowHeight="18768" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
   <si>
     <t>attributeName</t>
   </si>
@@ -295,13 +295,19 @@
   </si>
   <si>
     <t>Project associated to the cruise</t>
+  </si>
+  <si>
+    <t>NES-LTER</t>
+  </si>
+  <si>
+    <t>Information Manager</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,6 +318,21 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -335,11 +356,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -348,10 +371,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -631,18 +659,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="62.77734375" style="1" customWidth="1"/>
-    <col min="3" max="8" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.41796875" customWidth="1"/>
+    <col min="2" max="2" width="62.7890625" style="1" customWidth="1"/>
+    <col min="3" max="8" width="20.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -665,7 +693,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -682,7 +710,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -693,7 +721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -707,7 +735,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -718,7 +746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -729,7 +757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -740,7 +768,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -757,7 +785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -777,7 +805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -797,7 +825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -808,7 +836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -833,9 +861,9 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -846,7 +874,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -857,7 +885,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -868,7 +896,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -879,7 +907,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -899,103 +927,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I2" t="s">
+      <c r="E3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J3" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1018,7 +1055,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1047,9 +1084,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>89</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="D6" t="s">
         <v>31</v>
@@ -1072,7 +1112,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{0FC6BA44-FFCE-489C-AE09-C48BCA4C2F5A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1086,12 +1127,12 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="22.6640625" customWidth="1"/>
+    <col min="1" max="2" width="22.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1099,7 +1140,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -1107,7 +1148,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -1115,7 +1156,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>81</v>
       </c>
@@ -1123,7 +1164,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>82</v>
       </c>
@@ -1131,7 +1172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -1139,7 +1180,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -1147,7 +1188,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -1155,7 +1196,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>84</v>
       </c>
@@ -1163,7 +1204,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
adding NES-LTER organization as creator
</commit_message>
<xml_diff>
--- a/nes-lter-events-transect-info.xlsx
+++ b/nes-lter-events-transect-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfutrelle\Documents\GitHub\nes-lter-events-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF45EB3-1837-42F1-9A37-FAD4AB724896}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50F9DD3-2DA9-46E6-A994-85AA4912DE06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29118" yWindow="1038" windowWidth="25098" windowHeight="18768" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="91">
   <si>
     <t>attributeName</t>
   </si>
@@ -925,10 +925,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -969,34 +969,22 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1013,14 +1001,14 @@
       <c r="D3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>31</v>
@@ -1032,47 +1020,50 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="E4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" t="s">
-        <v>52</v>
+      <c r="E5" t="s">
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H5" t="s">
         <v>31</v>
@@ -1084,21 +1075,24 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>90</v>
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
       </c>
       <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="s">
-        <v>38</v>
+      <c r="E6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H6" t="s">
         <v>31</v>
@@ -1110,10 +1104,36 @@
         <v>35</v>
       </c>
     </row>
+    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
-    <hyperlink ref="E5" r:id="rId2" xr:uid="{0FC6BA44-FFCE-489C-AE09-C48BCA4C2F5A}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{0FC6BA44-FFCE-489C-AE09-C48BCA4C2F5A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
edited title, attribute definition and missing value code, methods
</commit_message>
<xml_diff>
--- a/nes-lter-events-transect-info.xlsx
+++ b/nes-lter-events-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfutrelle\Documents\GitHub\nes-lter-events-transect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-events-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50F9DD3-2DA9-46E6-A994-85AA4912DE06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F03521E-9913-4985-A494-867EE66E4B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29118" yWindow="1038" windowWidth="25098" windowHeight="18768" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="91">
   <si>
     <t>attributeName</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Cast</t>
   </si>
   <si>
-    <t>CTD rosette cast number or other designation</t>
-  </si>
-  <si>
     <t>Latitude</t>
   </si>
   <si>
@@ -301,6 +298,9 @@
   </si>
   <si>
     <t>Information Manager</t>
+  </si>
+  <si>
+    <t>Cast number count for Instrument associated with event if applicable</t>
   </si>
 </sst>
 </file>
@@ -659,18 +659,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.41796875" customWidth="1"/>
-    <col min="2" max="2" width="62.7890625" style="1" customWidth="1"/>
-    <col min="3" max="8" width="20.41796875" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="62.77734375" style="1" customWidth="1"/>
+    <col min="3" max="8" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +693,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -710,7 +710,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -720,8 +720,14 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -734,8 +740,14 @@
       <c r="E4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -745,8 +757,14 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -756,8 +774,14 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -768,29 +792,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>66</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -805,12 +823,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -825,26 +843,32 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -861,9 +885,9 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -874,7 +898,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -885,7 +909,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -896,26 +920,26 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>41</v>
       </c>
       <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
         <v>74</v>
       </c>
-      <c r="C4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>41</v>
       </c>
       <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
         <v>76</v>
-      </c>
-      <c r="C5" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -927,16 +951,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -968,7 +992,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>31</v>
       </c>
@@ -988,7 +1012,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
@@ -1020,7 +1044,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
@@ -1052,7 +1076,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1075,7 +1099,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1104,12 +1128,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="D7" t="s">
         <v>31</v>
@@ -1147,12 +1171,12 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="22.68359375" customWidth="1"/>
+    <col min="1" max="2" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1160,73 +1184,73 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
calculate geo coord & fix personnel
</commit_message>
<xml_diff>
--- a/nes-lter-events-transect-info.xlsx
+++ b/nes-lter-events-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-events-transect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkoch\Desktop\LTER\nes-lter-events-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F03521E-9913-4985-A494-867EE66E4B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F9F1F3-044A-41FA-8C93-DB8DA4400DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1350" yWindow="2080" windowWidth="15070" windowHeight="9200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="99">
   <si>
     <t>attributeName</t>
   </si>
@@ -301,6 +301,30 @@
   </si>
   <si>
     <t>Cast number count for Instrument associated with event if applicable</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>dimensionless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA </t>
+  </si>
+  <si>
+    <t>E.</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Crockford</t>
+  </si>
+  <si>
+    <t>ecrockford@whoi.edu</t>
+  </si>
+  <si>
+    <t>0000-0002-2122-0462</t>
   </si>
 </sst>
 </file>
@@ -362,7 +386,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -373,7 +397,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -659,18 +682,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="62.77734375" style="1" customWidth="1"/>
-    <col min="3" max="8" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="62.81640625" style="1" customWidth="1"/>
+    <col min="3" max="8" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -704,13 +727,13 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -718,7 +741,10 @@
         <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -727,7 +753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -741,13 +767,13 @@
         <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -758,13 +784,13 @@
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -775,13 +801,13 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -792,7 +818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -803,7 +829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -823,7 +849,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -843,7 +869,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -854,7 +880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -885,9 +911,9 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -898,7 +924,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -909,7 +935,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -920,7 +946,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -931,7 +957,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -949,18 +975,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -992,7 +1018,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
         <v>31</v>
       </c>
@@ -1012,7 +1038,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
@@ -1044,7 +1070,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
@@ -1076,7 +1102,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1099,7 +1125,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1128,11 +1154,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>89</v>
       </c>
       <c r="D7" t="s">
@@ -1151,6 +1177,38 @@
         <v>34</v>
       </c>
       <c r="J7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1171,12 +1229,12 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="22.6640625" customWidth="1"/>
+    <col min="1" max="2" width="22.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1184,7 +1242,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -1192,7 +1250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -1200,7 +1258,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>80</v>
       </c>
@@ -1208,7 +1266,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>81</v>
       </c>
@@ -1216,7 +1274,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -1224,7 +1282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -1232,7 +1290,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -1240,7 +1298,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>83</v>
       </c>
@@ -1248,7 +1306,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
updated data table and datetime format to handle midnights
</commit_message>
<xml_diff>
--- a/nes-lter-events-transect-info.xlsx
+++ b/nes-lter-events-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmorkeski\Documents\nes-lter-events-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E853CB13-2FEE-403E-BC51-7CDEBD19C85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AC8783-E90D-4518-AD40-68499C62464C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="105">
   <si>
     <t>attributeName</t>
   </si>
@@ -147,9 +147,6 @@
     <t>contact</t>
   </si>
   <si>
-    <t>metadataProvider</t>
-  </si>
-  <si>
     <t>project_id</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>MIT-WHOI Joint Program</t>
   </si>
   <si>
-    <t>YYYY-MM-DD hh:mm:ss</t>
-  </si>
-  <si>
     <t>Joe</t>
   </si>
   <si>
@@ -291,12 +285,6 @@
     <t>Project associated to the cruise</t>
   </si>
   <si>
-    <t>NES-LTER</t>
-  </si>
-  <si>
-    <t>Information Manager</t>
-  </si>
-  <si>
     <t>Cast number count for Instrument associated with event if applicable</t>
   </si>
   <si>
@@ -348,13 +336,13 @@
     <t>OCE-2322680</t>
   </si>
   <si>
-    <t>OCE-2322681</t>
-  </si>
-  <si>
     <t>OCE-2322682</t>
   </si>
   <si>
     <t>OCE-2322683</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DDThh:mm:ssZ</t>
   </si>
 </sst>
 </file>
@@ -718,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -754,7 +742,7 @@
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -763,24 +751,24 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -791,19 +779,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -811,44 +799,44 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -856,10 +844,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -867,10 +855,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -887,10 +875,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -907,10 +895,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -918,13 +906,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F12" t="s">
         <v>13</v>
@@ -954,54 +942,54 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1011,10 +999,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1071,7 +1059,7 @@
         <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1103,7 +1091,7 @@
         <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1126,7 +1114,7 @@
         <v>33</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>31</v>
@@ -1135,7 +1123,7 @@
         <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1158,27 +1146,27 @@
         <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
         <v>31</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
         <v>50</v>
-      </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" t="s">
-        <v>52</v>
       </c>
       <c r="H6" t="s">
         <v>31</v>
@@ -1187,24 +1175,30 @@
         <v>34</v>
       </c>
       <c r="J6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
       </c>
       <c r="D7" t="s">
         <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>92</v>
+      </c>
+      <c r="F7" t="s">
+        <v>93</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -1213,14 +1207,11 @@
         <v>34</v>
       </c>
       <c r="J7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" t="s">
         <v>94</v>
       </c>
       <c r="C8" t="s">
@@ -1229,14 +1220,11 @@
       <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F8" t="s">
-        <v>97</v>
-      </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
         <v>31</v>
@@ -1245,33 +1233,7 @@
         <v>34</v>
       </c>
       <c r="J8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1279,7 +1241,7 @@
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
     <hyperlink ref="E6" r:id="rId2" xr:uid="{0FC6BA44-FFCE-489C-AE09-C48BCA4C2F5A}"/>
-    <hyperlink ref="E9" r:id="rId3" xr:uid="{6E99CB3D-8C51-40BF-98C3-41F04017D697}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{6E99CB3D-8C51-40BF-98C3-41F04017D697}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1308,7 +1270,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -1316,7 +1278,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -1324,7 +1286,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -1332,7 +1294,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -1340,7 +1302,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -1348,7 +1310,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -1356,7 +1318,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -1364,7 +1326,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
@@ -1372,7 +1334,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>

</xml_diff>